<commit_message>
fix upload antibiotic entry view
</commit_message>
<xml_diff>
--- a/apps/template_docs/Antibiotics.xlsx
+++ b/apps/template_docs/Antibiotics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REFERRED_DB_052325\REFERRED_DB\apps\template_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B1C18E-A840-4A9D-A7C3-D39450BA0374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227B2FC7-5B56-4DCF-A646-5AF1431098C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3114,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H325"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>